<commit_message>
Update PluralityBook Ownership List.xlsx
Updating ownership excel
</commit_message>
<xml_diff>
--- a/PluralityBook Ownership List.xlsx
+++ b/PluralityBook Ownership List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jentenmann\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jentenmann\Documents\GitHub\plurality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EE0A2B-F7DD-423D-B153-2F86B62708DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C673FF8-9956-4AD3-8B7C-6BB236C3EA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{93E96F9A-2926-4F9E-A5CD-C3A950EE7EC3}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>Japanese</t>
   </si>
   <si>
-    <t>akinori.oyama@gmail.com</t>
-  </si>
-  <si>
     <t>Legal/Governance/Money Management</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Website/Book Visuals</t>
+  </si>
+  <si>
+    <t>akinori.oyama@akinorioyama.com</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
     <col min="3" max="3" width="11.81640625" customWidth="1"/>
     <col min="4" max="4" width="11.54296875" customWidth="1"/>
     <col min="5" max="5" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.1796875" bestFit="1" customWidth="1"/>
@@ -541,10 +541,10 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
         <v>1</v>
@@ -558,10 +558,10 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.35">
@@ -572,10 +572,10 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -583,76 +583,75 @@
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{3707B658-AD94-4A2C-864D-C942CEBADD7C}"/>
-    <hyperlink ref="F7" r:id="rId2" xr:uid="{34CEFB13-188C-4E9A-8866-4E117DD51C16}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{56989200-4E14-4B0C-969D-E6CF498F36C8}"/>
-    <hyperlink ref="F12" r:id="rId4" xr:uid="{038C9180-BE7F-4003-A2A7-3F32C32E679C}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{56989200-4E14-4B0C-969D-E6CF498F36C8}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{038C9180-BE7F-4003-A2A7-3F32C32E679C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>